<commit_message>
Fixed Investment Template and updated
</commit_message>
<xml_diff>
--- a/Pages/Projects/Graph Calculator.xlsx
+++ b/Pages/Projects/Graph Calculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bret\OneDrive\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bret\OneDrive\Website\bretallinott.github.io\Pages\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_AE4556612AB3EA2D9229781B9EB1C5B6BD18DAA0" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9D51149B-E672-4052-8395-98E122AA8F2D}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_AE4556612AB3EA2D9229781B9EB1C5B6BD18DAA0" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EFB5DAB5-6EB9-4ECF-B14E-9FC0D16F8AEB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,25 +354,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>-3</c:v>
+                  <c:v>-1.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2</c:v>
+                  <c:v>-1.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>-0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,28 +384,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-27</c:v>
+                  <c:v>-76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1134,7 +1134,7 @@
   <dimension ref="A1:Z53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G23" si="1">D3-$R$27</f>
-        <v>-10</v>
+        <v>-13</v>
       </c>
       <c r="H3">
         <f>E3</f>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J23" si="2">G3/$R$29</f>
-        <v>-10</v>
+        <v>-3.25</v>
       </c>
       <c r="K3">
         <f>H3</f>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M23" si="3">J3*$R$31</f>
-        <v>-10</v>
+        <v>-3.25</v>
       </c>
       <c r="N3">
         <f>K3</f>
@@ -1277,35 +1277,35 @@
       </c>
       <c r="P3">
         <f>M3</f>
-        <v>-10</v>
+        <v>-3.25</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q23" si="4">N3*$R$33</f>
-        <v>-1000</v>
+        <v>-3000</v>
       </c>
       <c r="S3">
         <f>P3</f>
-        <v>-10</v>
+        <v>-3.25</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T23" si="5">Q3*$R$35</f>
-        <v>-1000</v>
+        <v>-3000</v>
       </c>
       <c r="V3">
         <f>S3</f>
-        <v>-10</v>
+        <v>-3.25</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W23" si="6">T3+$R$37</f>
-        <v>-1000</v>
+        <v>-2995</v>
       </c>
       <c r="Y3" s="1">
         <f>V3</f>
-        <v>-10</v>
+        <v>-3.25</v>
       </c>
       <c r="Z3" s="1">
         <f>W3</f>
-        <v>-1000</v>
+        <v>-2995</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>-9</v>
+        <v>-12</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H23" si="9">E4</f>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K23" si="10">H4</f>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="M4">
         <f t="shared" si="3"/>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N23" si="11">K4</f>
@@ -1350,35 +1350,35 @@
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P23" si="12">M4</f>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="Q4">
         <f t="shared" si="4"/>
-        <v>-729</v>
+        <v>-2187</v>
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S23" si="13">P4</f>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="T4">
         <f t="shared" si="5"/>
-        <v>-729</v>
+        <v>-2187</v>
       </c>
       <c r="V4">
         <f t="shared" ref="V4:V23" si="14">S4</f>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="W4">
         <f t="shared" si="6"/>
-        <v>-729</v>
+        <v>-2182</v>
       </c>
       <c r="Y4" s="1">
         <f t="shared" ref="Y4:Y23" si="15">V4</f>
-        <v>-9</v>
+        <v>-3</v>
       </c>
       <c r="Z4" s="1">
         <f t="shared" ref="Z4:Z23" si="16">W4</f>
-        <v>-729</v>
+        <v>-2182</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>-8</v>
+        <v>-11</v>
       </c>
       <c r="H5">
         <f t="shared" si="9"/>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>-8</v>
+        <v>-2.75</v>
       </c>
       <c r="K5">
         <f t="shared" si="10"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>-8</v>
+        <v>-2.75</v>
       </c>
       <c r="N5">
         <f t="shared" si="11"/>
@@ -1423,35 +1423,35 @@
       </c>
       <c r="P5">
         <f t="shared" si="12"/>
-        <v>-8</v>
+        <v>-2.75</v>
       </c>
       <c r="Q5">
         <f t="shared" si="4"/>
-        <v>-512</v>
+        <v>-1536</v>
       </c>
       <c r="S5">
         <f t="shared" si="13"/>
-        <v>-8</v>
+        <v>-2.75</v>
       </c>
       <c r="T5">
         <f t="shared" si="5"/>
-        <v>-512</v>
+        <v>-1536</v>
       </c>
       <c r="V5">
         <f t="shared" si="14"/>
-        <v>-8</v>
+        <v>-2.75</v>
       </c>
       <c r="W5">
         <f t="shared" si="6"/>
-        <v>-512</v>
+        <v>-1531</v>
       </c>
       <c r="Y5" s="1">
         <f t="shared" si="15"/>
-        <v>-8</v>
+        <v>-2.75</v>
       </c>
       <c r="Z5" s="1">
         <f t="shared" si="16"/>
-        <v>-512</v>
+        <v>-1531</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="H6">
         <f t="shared" si="9"/>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="K6">
         <f t="shared" si="10"/>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="N6">
         <f t="shared" si="11"/>
@@ -1496,35 +1496,35 @@
       </c>
       <c r="P6">
         <f t="shared" si="12"/>
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
-        <v>-343</v>
+        <v>-1029</v>
       </c>
       <c r="S6">
         <f t="shared" si="13"/>
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="T6">
         <f t="shared" si="5"/>
-        <v>-343</v>
+        <v>-1029</v>
       </c>
       <c r="V6">
         <f t="shared" si="14"/>
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="W6">
         <f t="shared" si="6"/>
-        <v>-343</v>
+        <v>-1024</v>
       </c>
       <c r="Y6" s="1">
         <f t="shared" si="15"/>
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="Z6" s="1">
         <f t="shared" si="16"/>
-        <v>-343</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-9</v>
       </c>
       <c r="H7">
         <f t="shared" si="9"/>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>-6</v>
+        <v>-2.25</v>
       </c>
       <c r="K7">
         <f t="shared" si="10"/>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>-6</v>
+        <v>-2.25</v>
       </c>
       <c r="N7">
         <f t="shared" si="11"/>
@@ -1569,35 +1569,35 @@
       </c>
       <c r="P7">
         <f t="shared" si="12"/>
-        <v>-6</v>
+        <v>-2.25</v>
       </c>
       <c r="Q7">
         <f t="shared" si="4"/>
-        <v>-216</v>
+        <v>-648</v>
       </c>
       <c r="S7">
         <f t="shared" si="13"/>
-        <v>-6</v>
+        <v>-2.25</v>
       </c>
       <c r="T7">
         <f t="shared" si="5"/>
-        <v>-216</v>
+        <v>-648</v>
       </c>
       <c r="V7">
         <f t="shared" si="14"/>
-        <v>-6</v>
+        <v>-2.25</v>
       </c>
       <c r="W7">
         <f t="shared" si="6"/>
-        <v>-216</v>
+        <v>-643</v>
       </c>
       <c r="Y7" s="1">
         <f t="shared" si="15"/>
-        <v>-6</v>
+        <v>-2.25</v>
       </c>
       <c r="Z7" s="1">
         <f t="shared" si="16"/>
-        <v>-216</v>
+        <v>-643</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="H8">
         <f t="shared" si="9"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="K8">
         <f t="shared" si="10"/>
@@ -1634,7 +1634,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="N8">
         <f t="shared" si="11"/>
@@ -1642,35 +1642,35 @@
       </c>
       <c r="P8">
         <f t="shared" si="12"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="Q8">
         <f t="shared" si="4"/>
-        <v>-125</v>
+        <v>-375</v>
       </c>
       <c r="S8">
         <f t="shared" si="13"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="T8">
         <f t="shared" si="5"/>
-        <v>-125</v>
+        <v>-375</v>
       </c>
       <c r="V8">
         <f t="shared" si="14"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>-125</v>
+        <v>-370</v>
       </c>
       <c r="Y8" s="1">
         <f t="shared" si="15"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="Z8" s="1">
         <f t="shared" si="16"/>
-        <v>-125</v>
+        <v>-370</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>-7</v>
       </c>
       <c r="H9">
         <f t="shared" si="9"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="J9">
         <f t="shared" si="2"/>
-        <v>-4</v>
+        <v>-1.75</v>
       </c>
       <c r="K9">
         <f t="shared" si="10"/>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>-4</v>
+        <v>-1.75</v>
       </c>
       <c r="N9">
         <f t="shared" si="11"/>
@@ -1715,35 +1715,35 @@
       </c>
       <c r="P9">
         <f t="shared" si="12"/>
-        <v>-4</v>
+        <v>-1.75</v>
       </c>
       <c r="Q9">
         <f t="shared" si="4"/>
-        <v>-64</v>
+        <v>-192</v>
       </c>
       <c r="S9">
         <f t="shared" si="13"/>
-        <v>-4</v>
+        <v>-1.75</v>
       </c>
       <c r="T9">
         <f t="shared" si="5"/>
-        <v>-64</v>
+        <v>-192</v>
       </c>
       <c r="V9">
         <f t="shared" si="14"/>
-        <v>-4</v>
+        <v>-1.75</v>
       </c>
       <c r="W9">
         <f t="shared" si="6"/>
-        <v>-64</v>
+        <v>-187</v>
       </c>
       <c r="Y9" s="1">
         <f t="shared" si="15"/>
-        <v>-4</v>
+        <v>-1.75</v>
       </c>
       <c r="Z9" s="1">
         <f t="shared" si="16"/>
-        <v>-64</v>
+        <v>-187</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="H10">
         <f t="shared" si="9"/>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>-1.5</v>
       </c>
       <c r="K10">
         <f t="shared" si="10"/>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>-1.5</v>
       </c>
       <c r="N10">
         <f t="shared" si="11"/>
@@ -1788,35 +1788,35 @@
       </c>
       <c r="P10">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-1.5</v>
       </c>
       <c r="Q10">
         <f t="shared" si="4"/>
-        <v>-27</v>
+        <v>-81</v>
       </c>
       <c r="S10">
         <f t="shared" si="13"/>
-        <v>-3</v>
+        <v>-1.5</v>
       </c>
       <c r="T10">
         <f t="shared" si="5"/>
-        <v>-27</v>
+        <v>-81</v>
       </c>
       <c r="V10">
         <f t="shared" si="14"/>
-        <v>-3</v>
+        <v>-1.5</v>
       </c>
       <c r="W10">
         <f t="shared" si="6"/>
-        <v>-27</v>
+        <v>-76</v>
       </c>
       <c r="Y10" s="1">
         <f t="shared" si="15"/>
-        <v>-3</v>
+        <v>-1.5</v>
       </c>
       <c r="Z10" s="1">
         <f t="shared" si="16"/>
-        <v>-27</v>
+        <v>-76</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="H11">
         <f t="shared" si="9"/>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>-1.25</v>
       </c>
       <c r="K11">
         <f t="shared" si="10"/>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>-1.25</v>
       </c>
       <c r="N11">
         <f t="shared" si="11"/>
@@ -1861,35 +1861,35 @@
       </c>
       <c r="P11">
         <f t="shared" si="12"/>
-        <v>-2</v>
+        <v>-1.25</v>
       </c>
       <c r="Q11">
         <f t="shared" si="4"/>
-        <v>-8</v>
+        <v>-24</v>
       </c>
       <c r="S11">
         <f t="shared" si="13"/>
-        <v>-2</v>
+        <v>-1.25</v>
       </c>
       <c r="T11">
         <f t="shared" si="5"/>
-        <v>-8</v>
+        <v>-24</v>
       </c>
       <c r="V11">
         <f t="shared" si="14"/>
-        <v>-2</v>
+        <v>-1.25</v>
       </c>
       <c r="W11">
         <f t="shared" si="6"/>
-        <v>-8</v>
+        <v>-19</v>
       </c>
       <c r="Y11" s="1">
         <f t="shared" si="15"/>
-        <v>-2</v>
+        <v>-1.25</v>
       </c>
       <c r="Z11" s="1">
         <f t="shared" si="16"/>
-        <v>-8</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="H12">
         <f t="shared" si="9"/>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="Q12">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="S12">
         <f t="shared" si="13"/>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="T12">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="V12">
         <f t="shared" si="14"/>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="W12">
         <f t="shared" si="6"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Y12" s="1">
         <f t="shared" si="15"/>
@@ -1962,7 +1962,7 @@
       </c>
       <c r="Z12" s="1">
         <f t="shared" si="16"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -1983,7 +1983,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="H13">
         <f t="shared" si="9"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="J13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="K13">
         <f t="shared" si="10"/>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="M13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="N13">
         <f t="shared" si="11"/>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="P13">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Q13">
         <f t="shared" si="4"/>
@@ -2015,7 +2015,7 @@
       </c>
       <c r="S13">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="T13">
         <f t="shared" si="5"/>
@@ -2023,19 +2023,19 @@
       </c>
       <c r="V13">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="W13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y13" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Z13" s="1">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="H14">
         <f t="shared" si="9"/>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="K14">
         <f t="shared" si="10"/>
@@ -2072,7 +2072,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="N14">
         <f t="shared" si="11"/>
@@ -2080,35 +2080,35 @@
       </c>
       <c r="P14">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="Q14">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S14">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="T14">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V14">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="W14">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Y14" s="1">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z14" s="1">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="H15">
         <f t="shared" si="9"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="J15">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>-0.25</v>
       </c>
       <c r="K15">
         <f t="shared" si="10"/>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>-0.25</v>
       </c>
       <c r="N15">
         <f t="shared" si="11"/>
@@ -2153,35 +2153,35 @@
       </c>
       <c r="P15">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>-0.25</v>
       </c>
       <c r="Q15">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="S15">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>-0.25</v>
       </c>
       <c r="T15">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="V15">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>-0.25</v>
       </c>
       <c r="W15">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="Y15" s="1">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>-0.25</v>
       </c>
       <c r="Z15" s="1">
         <f t="shared" si="16"/>
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" si="9"/>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="J16">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <f t="shared" si="10"/>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N16">
         <f t="shared" si="11"/>
@@ -2226,35 +2226,35 @@
       </c>
       <c r="P16">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q16">
         <f t="shared" si="4"/>
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="S16">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="V16">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W16">
         <f t="shared" si="6"/>
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="Y16" s="1">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="1">
         <f t="shared" si="16"/>
-        <v>27</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <f t="shared" si="9"/>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="J17">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="K17">
         <f t="shared" si="10"/>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="N17">
         <f t="shared" si="11"/>
@@ -2299,35 +2299,35 @@
       </c>
       <c r="P17">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="Q17">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>192</v>
       </c>
       <c r="S17">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="T17">
         <f t="shared" si="5"/>
-        <v>64</v>
+        <v>192</v>
       </c>
       <c r="V17">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="W17">
         <f t="shared" si="6"/>
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="Y17" s="1">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>0.25</v>
       </c>
       <c r="Z17" s="1">
         <f t="shared" si="16"/>
-        <v>64</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -2348,7 +2348,7 @@
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <f t="shared" si="9"/>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="J18">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="K18">
         <f t="shared" si="10"/>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="M18">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="N18">
         <f t="shared" si="11"/>
@@ -2372,35 +2372,35 @@
       </c>
       <c r="P18">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="Q18">
         <f t="shared" si="4"/>
-        <v>125</v>
+        <v>375</v>
       </c>
       <c r="S18">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="T18">
         <f t="shared" si="5"/>
-        <v>125</v>
+        <v>375</v>
       </c>
       <c r="V18">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="W18">
         <f t="shared" si="6"/>
-        <v>125</v>
+        <v>380</v>
       </c>
       <c r="Y18" s="1">
         <f t="shared" si="15"/>
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="Z18" s="1">
         <f t="shared" si="16"/>
-        <v>125</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H19">
         <f t="shared" si="9"/>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>0.75</v>
       </c>
       <c r="K19">
         <f t="shared" si="10"/>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="M19">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>0.75</v>
       </c>
       <c r="N19">
         <f t="shared" si="11"/>
@@ -2445,35 +2445,35 @@
       </c>
       <c r="P19">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>0.75</v>
       </c>
       <c r="Q19">
         <f t="shared" si="4"/>
-        <v>216</v>
+        <v>648</v>
       </c>
       <c r="S19">
         <f t="shared" si="13"/>
-        <v>6</v>
+        <v>0.75</v>
       </c>
       <c r="T19">
         <f t="shared" si="5"/>
-        <v>216</v>
+        <v>648</v>
       </c>
       <c r="V19">
         <f t="shared" si="14"/>
-        <v>6</v>
+        <v>0.75</v>
       </c>
       <c r="W19">
         <f t="shared" si="6"/>
-        <v>216</v>
+        <v>653</v>
       </c>
       <c r="Y19" s="1">
         <f t="shared" si="15"/>
-        <v>6</v>
+        <v>0.75</v>
       </c>
       <c r="Z19" s="1">
         <f t="shared" si="16"/>
-        <v>216</v>
+        <v>653</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H20">
         <f t="shared" si="9"/>
@@ -2502,7 +2502,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <f t="shared" si="10"/>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="M20">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N20">
         <f t="shared" si="11"/>
@@ -2518,35 +2518,35 @@
       </c>
       <c r="P20">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q20">
         <f t="shared" si="4"/>
-        <v>343</v>
+        <v>1029</v>
       </c>
       <c r="S20">
         <f t="shared" si="13"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="T20">
         <f t="shared" si="5"/>
-        <v>343</v>
+        <v>1029</v>
       </c>
       <c r="V20">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="W20">
         <f t="shared" si="6"/>
-        <v>343</v>
+        <v>1034</v>
       </c>
       <c r="Y20" s="1">
         <f t="shared" si="15"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Z20" s="1">
         <f t="shared" si="16"/>
-        <v>343</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H21">
         <f t="shared" si="9"/>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>1.25</v>
       </c>
       <c r="K21">
         <f t="shared" si="10"/>
@@ -2583,7 +2583,7 @@
       </c>
       <c r="M21">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>1.25</v>
       </c>
       <c r="N21">
         <f t="shared" si="11"/>
@@ -2591,35 +2591,35 @@
       </c>
       <c r="P21">
         <f t="shared" si="12"/>
-        <v>8</v>
+        <v>1.25</v>
       </c>
       <c r="Q21">
         <f t="shared" si="4"/>
-        <v>512</v>
+        <v>1536</v>
       </c>
       <c r="S21">
         <f t="shared" si="13"/>
-        <v>8</v>
+        <v>1.25</v>
       </c>
       <c r="T21">
         <f t="shared" si="5"/>
-        <v>512</v>
+        <v>1536</v>
       </c>
       <c r="V21">
         <f t="shared" si="14"/>
-        <v>8</v>
+        <v>1.25</v>
       </c>
       <c r="W21">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>1541</v>
       </c>
       <c r="Y21" s="1">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>1.25</v>
       </c>
       <c r="Z21" s="1">
         <f t="shared" si="16"/>
-        <v>512</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H22">
         <f t="shared" si="9"/>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="K22">
         <f t="shared" si="10"/>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="M22">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="N22">
         <f t="shared" si="11"/>
@@ -2664,35 +2664,35 @@
       </c>
       <c r="P22">
         <f t="shared" si="12"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="Q22">
         <f t="shared" si="4"/>
-        <v>729</v>
+        <v>2187</v>
       </c>
       <c r="S22">
         <f t="shared" si="13"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="T22">
         <f t="shared" si="5"/>
-        <v>729</v>
+        <v>2187</v>
       </c>
       <c r="V22">
         <f t="shared" si="14"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="W22">
         <f t="shared" si="6"/>
-        <v>729</v>
+        <v>2192</v>
       </c>
       <c r="Y22" s="1">
         <f t="shared" si="15"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="Z22" s="1">
         <f t="shared" si="16"/>
-        <v>729</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H23">
         <f t="shared" si="9"/>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="J23">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1.75</v>
       </c>
       <c r="K23">
         <f t="shared" si="10"/>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="M23">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>1.75</v>
       </c>
       <c r="N23">
         <f t="shared" si="11"/>
@@ -2737,35 +2737,35 @@
       </c>
       <c r="P23">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>1.75</v>
       </c>
       <c r="Q23">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="S23">
         <f t="shared" si="13"/>
-        <v>10</v>
+        <v>1.75</v>
       </c>
       <c r="T23">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="V23">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>1.75</v>
       </c>
       <c r="W23">
         <f t="shared" si="6"/>
-        <v>1000</v>
+        <v>3005</v>
       </c>
       <c r="Y23" s="1">
         <f t="shared" si="15"/>
-        <v>10</v>
+        <v>1.75</v>
       </c>
       <c r="Z23" s="1">
         <f t="shared" si="16"/>
-        <v>1000</v>
+        <v>3005</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -2796,7 +2796,7 @@
         <v>10</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S27" t="s">
         <v>22</v>
@@ -2817,7 +2817,7 @@
         <v>11</v>
       </c>
       <c r="R29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S29" t="s">
         <v>17</v>
@@ -2847,11 +2847,11 @@
       </c>
       <c r="X31">
         <f>Y53</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="Y31">
         <f>Z53</f>
-        <v>27</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -2862,7 +2862,7 @@
         <v>13</v>
       </c>
       <c r="R33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S33" t="s">
         <v>18</v>
@@ -2890,7 +2890,7 @@
         <v>15</v>
       </c>
       <c r="R37">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
@@ -2997,7 +2997,7 @@
       </c>
       <c r="G53">
         <f t="shared" ref="G53" si="18">D53-$R$27</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="H53">
         <f>E53</f>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="J53">
         <f t="shared" ref="J53" si="19">G53/$R$29</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="K53">
         <f>H53</f>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="M53">
         <f t="shared" ref="M53" si="20">J53*$R$31</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="N53">
         <f>K53</f>
@@ -3021,35 +3021,35 @@
       </c>
       <c r="P53">
         <f>M53</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="Q53">
         <f t="shared" ref="Q53" si="21">N53*$R$33</f>
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="S53">
         <f>P53</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="T53">
         <f t="shared" ref="T53" si="22">Q53*$R$35</f>
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="V53">
         <f>S53</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="W53">
         <f t="shared" ref="W53" si="23">T53+$R$37</f>
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="Y53">
         <f>V53</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z53">
         <f>W53</f>
-        <v>27</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>